<commit_message>
Evaluation: don't include hashes in optimum
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/dev/cl/byzantine-eventual/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3071C664-57F1-2742-A3B4-2F812EBB21A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153B7CDF-CE15-384C-A18A-96175D0E35B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-9640" windowWidth="22640" windowHeight="31420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>updates/sec/process</t>
   </si>
@@ -85,11 +85,26 @@
   <si>
     <t>v2 overhead bytes/reconciliation</t>
   </si>
+  <si>
+    <t>v2 overhead</t>
+  </si>
+  <si>
+    <t>payload kb/sec</t>
+  </si>
+  <si>
+    <t>v1 total kb/sec</t>
+  </si>
+  <si>
+    <t>v2 total kb/sec</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -567,10 +582,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -658,7 +674,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>v1 total bytes/sec</c:v>
+                  <c:v>v1 total kb/sec</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -722,25 +738,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1289</c:v>
+                  <c:v>1.29836</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4180</c:v>
+                  <c:v>9.3044799999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6572</c:v>
+                  <c:v>15.884</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13580</c:v>
+                  <c:v>34.617440000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26094</c:v>
+                  <c:v>67.03904</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38408</c:v>
+                  <c:v>99.260480000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50919</c:v>
+                  <c:v>131.67792</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -761,7 +777,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>v2 total bytes/sec</c:v>
+                  <c:v>v2 total kb/sec</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -825,25 +841,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1665</c:v>
+                  <c:v>2.2742799999999899</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4296</c:v>
+                  <c:v>10.0016</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5297</c:v>
+                  <c:v>14.8888</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8329</c:v>
+                  <c:v>28.445360000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14542</c:v>
+                  <c:v>52.64264</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20763</c:v>
+                  <c:v>76.852239999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26983</c:v>
+                  <c:v>101.0592</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -864,7 +880,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>payload bytes/sec</c:v>
+                  <c:v>payload kb/sec</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -928,25 +944,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>1.2E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1200</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2400</c:v>
+                  <c:v>9.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5988</c:v>
+                  <c:v>23.952000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11986</c:v>
+                  <c:v>47.944000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17982</c:v>
+                  <c:v>71.927999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23978</c:v>
+                  <c:v>95.912000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1129,7 +1145,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB" sz="1200"/>
-                  <a:t>network bytes transferred/sec</a:t>
+                  <a:t>network kB transferred/sec</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3270,11 +3286,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3290,15 +3304,15 @@
     <col min="15" max="15" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -3307,7 +3321,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
@@ -3333,16 +3347,19 @@
       <c r="O1" t="s">
         <v>17</v>
       </c>
+      <c r="P1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="C2">
-        <v>1289</v>
+        <v>1.29836</v>
       </c>
       <c r="D2">
         <v>2.0099999999999998</v>
@@ -3351,10 +3368,10 @@
         <v>1.0049999999999999</v>
       </c>
       <c r="F2">
-        <v>1665</v>
+        <v>2.2742799999999899</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -3373,22 +3390,26 @@
       </c>
       <c r="N2" s="1">
         <f>(C2/B2)-1</f>
-        <v>428.66666666666669</v>
+        <v>107.19666666666666</v>
       </c>
       <c r="O2">
         <f>(F2-B2)/6</f>
-        <v>277</v>
+        <v>0.37704666666666498</v>
+      </c>
+      <c r="P2" s="3">
+        <f>(F2/B2)-1</f>
+        <v>188.52333333333249</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1200</v>
+        <v>4.8</v>
       </c>
       <c r="C3">
-        <v>4180</v>
+        <v>9.3044799999999999</v>
       </c>
       <c r="D3">
         <v>4.6666666666666599</v>
@@ -3397,10 +3418,10 @@
         <v>1.6666666666666601</v>
       </c>
       <c r="F3">
-        <v>4296</v>
+        <v>10.0016</v>
       </c>
       <c r="G3">
-        <v>2.0266666666666602</v>
+        <v>4.0266666666666602</v>
       </c>
       <c r="H3">
         <v>1.0133333333333301</v>
@@ -3419,22 +3440,26 @@
       </c>
       <c r="N3" s="1">
         <f t="shared" ref="N3:N8" si="0">(C3/B3)-1</f>
-        <v>2.4833333333333334</v>
+        <v>0.93843333333333345</v>
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O8" si="1">(F3-B3)/6</f>
-        <v>516</v>
+        <v>0.86693333333333333</v>
+      </c>
+      <c r="P3" s="3">
+        <f t="shared" ref="P3:P8" si="2">(F3/B3)-1</f>
+        <v>1.0836666666666668</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2400</v>
+        <v>9.6</v>
       </c>
       <c r="C4">
-        <v>6572</v>
+        <v>15.884</v>
       </c>
       <c r="D4">
         <v>8</v>
@@ -3443,10 +3468,10 @@
         <v>2.5</v>
       </c>
       <c r="F4">
-        <v>5297</v>
+        <v>14.8888</v>
       </c>
       <c r="G4">
-        <v>2.0533333333333301</v>
+        <v>4.0533333333333301</v>
       </c>
       <c r="H4">
         <v>1.02666666666666</v>
@@ -3465,22 +3490,26 @@
       </c>
       <c r="N4" s="1">
         <f t="shared" si="0"/>
-        <v>1.7383333333333333</v>
+        <v>0.65458333333333352</v>
       </c>
       <c r="O4">
         <f t="shared" si="1"/>
-        <v>482.83333333333331</v>
+        <v>0.88146666666666673</v>
+      </c>
+      <c r="P4" s="3">
+        <f t="shared" si="2"/>
+        <v>0.55091666666666672</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>5988</v>
+        <v>23.952000000000002</v>
       </c>
       <c r="C5">
-        <v>13580</v>
+        <v>34.617440000000002</v>
       </c>
       <c r="D5">
         <v>16.64</v>
@@ -3489,10 +3518,10 @@
         <v>4.66</v>
       </c>
       <c r="F5">
-        <v>8329</v>
+        <v>28.445360000000001</v>
       </c>
       <c r="G5">
-        <v>2.11666666666666</v>
+        <v>4.11666666666666</v>
       </c>
       <c r="H5">
         <v>1.05833333333333</v>
@@ -3511,22 +3540,26 @@
       </c>
       <c r="N5" s="1">
         <f t="shared" si="0"/>
-        <v>1.2678690714762859</v>
+        <v>0.44528390113560445</v>
       </c>
       <c r="O5">
         <f t="shared" si="1"/>
-        <v>390.16666666666669</v>
+        <v>0.74889333333333319</v>
+      </c>
+      <c r="P5" s="3">
+        <f t="shared" si="2"/>
+        <v>0.18759853039412144</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>10</v>
       </c>
       <c r="B6">
-        <v>11986</v>
+        <v>47.944000000000003</v>
       </c>
       <c r="C6">
-        <v>26094</v>
+        <v>67.03904</v>
       </c>
       <c r="D6">
         <v>31.96</v>
@@ -3535,10 +3568,10 @@
         <v>8.49</v>
       </c>
       <c r="F6">
-        <v>14542</v>
+        <v>52.64264</v>
       </c>
       <c r="G6">
-        <v>2.0733333333333301</v>
+        <v>4.0733333333333297</v>
       </c>
       <c r="H6">
         <v>1.03666666666666</v>
@@ -3557,22 +3590,26 @@
       </c>
       <c r="N6" s="1">
         <f t="shared" si="0"/>
-        <v>1.1770398798598363</v>
+        <v>0.39827799098948757</v>
       </c>
       <c r="O6">
         <f t="shared" si="1"/>
-        <v>426</v>
+        <v>0.78310666666666628</v>
+      </c>
+      <c r="P6" s="3">
+        <f t="shared" si="2"/>
+        <v>9.8002669781411589E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>15</v>
       </c>
       <c r="B7">
-        <v>17982</v>
+        <v>71.927999999999997</v>
       </c>
       <c r="C7">
-        <v>38408</v>
+        <v>99.260480000000001</v>
       </c>
       <c r="D7">
         <v>46.626666666666601</v>
@@ -3581,10 +3618,10 @@
         <v>12.156666666666601</v>
       </c>
       <c r="F7">
-        <v>20763</v>
+        <v>76.852239999999995</v>
       </c>
       <c r="G7">
-        <v>2.07666666666666</v>
+        <v>4.07666666666666</v>
       </c>
       <c r="H7">
         <v>1.03833333333333</v>
@@ -3603,22 +3640,26 @@
       </c>
       <c r="N7" s="1">
         <f t="shared" si="0"/>
-        <v>1.1359136914692471</v>
+        <v>0.37999777555333125</v>
       </c>
       <c r="O7">
         <f t="shared" si="1"/>
-        <v>463.5</v>
+        <v>0.82070666666666625</v>
+      </c>
+      <c r="P7" s="3">
+        <f t="shared" si="2"/>
+        <v>6.8460682905127301E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20</v>
       </c>
       <c r="B8">
-        <v>23978</v>
+        <v>95.912000000000006</v>
       </c>
       <c r="C8">
-        <v>50919</v>
+        <v>131.67792</v>
       </c>
       <c r="D8">
         <v>61.946666666666601</v>
@@ -3627,10 +3668,10 @@
         <v>15.986666666666601</v>
       </c>
       <c r="F8">
-        <v>26983</v>
+        <v>101.0592</v>
       </c>
       <c r="G8">
-        <v>2.0666666666666602</v>
+        <v>4.0666666666666602</v>
       </c>
       <c r="H8">
         <v>1.0333333333333301</v>
@@ -3649,32 +3690,36 @@
       </c>
       <c r="N8" s="1">
         <f t="shared" si="0"/>
-        <v>1.1235716073066979</v>
+        <v>0.37290349487029761</v>
       </c>
       <c r="O8">
         <f t="shared" si="1"/>
-        <v>500.83333333333331</v>
+        <v>0.85786666666666633</v>
+      </c>
+      <c r="P8" s="3">
+        <f t="shared" si="2"/>
+        <v>5.3665860372007712E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I10" s="2">
         <f>SUM(I2:I8)/SUM($I2:$L8)</f>
         <v>0.97071428571428575</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" ref="J10:L10" si="2">SUM(J2:J8)/SUM($I2:$L8)</f>
+        <f t="shared" ref="J10:L10" si="3">SUM(J2:J8)/SUM($I2:$L8)</f>
         <v>2.9047619047619048E-2</v>
       </c>
       <c r="K10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.380952380952381E-4</v>
       </c>
       <c r="L10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -3727,10 +3772,10 @@
         <v>0</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C34">
-        <v>1289</v>
+        <v>1298</v>
       </c>
       <c r="D34">
         <v>2.0099999999999998</v>
@@ -3739,10 +3784,10 @@
         <v>1.0049999999999999</v>
       </c>
       <c r="F34">
-        <v>1665</v>
+        <v>2274</v>
       </c>
       <c r="G34">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -3765,10 +3810,10 @@
         <v>1</v>
       </c>
       <c r="B35">
-        <v>1200</v>
+        <v>4800</v>
       </c>
       <c r="C35">
-        <v>4180</v>
+        <v>9304</v>
       </c>
       <c r="D35">
         <v>4.6666666666666599</v>
@@ -3777,10 +3822,10 @@
         <v>1.6666666666666601</v>
       </c>
       <c r="F35">
-        <v>4289</v>
+        <v>10005</v>
       </c>
       <c r="G35">
-        <v>2.0166666666666599</v>
+        <v>4.0166666666666604</v>
       </c>
       <c r="H35">
         <v>1.00833333333333</v>
@@ -3803,10 +3848,10 @@
         <v>2</v>
       </c>
       <c r="B36">
-        <v>2400</v>
+        <v>9600</v>
       </c>
       <c r="C36">
-        <v>6572</v>
+        <v>15884</v>
       </c>
       <c r="D36">
         <v>8</v>
@@ -3815,10 +3860,10 @@
         <v>2.5</v>
       </c>
       <c r="F36">
-        <v>5296</v>
+        <v>14889</v>
       </c>
       <c r="G36">
-        <v>2.19</v>
+        <v>4.1900000000000004</v>
       </c>
       <c r="H36">
         <v>1.0916666666666599</v>
@@ -3841,10 +3886,10 @@
         <v>5</v>
       </c>
       <c r="B37">
-        <v>5988</v>
+        <v>23952</v>
       </c>
       <c r="C37">
-        <v>13580</v>
+        <v>34617</v>
       </c>
       <c r="D37">
         <v>16.64</v>
@@ -3853,10 +3898,10 @@
         <v>4.66</v>
       </c>
       <c r="F37">
-        <v>8345</v>
+        <v>28488</v>
       </c>
       <c r="G37">
-        <v>2.3966666666666598</v>
+        <v>4.3966666666666603</v>
       </c>
       <c r="H37">
         <v>1.17166666666666</v>
@@ -3879,10 +3924,10 @@
         <v>10</v>
       </c>
       <c r="B38">
-        <v>11986</v>
+        <v>47944</v>
       </c>
       <c r="C38">
-        <v>26094</v>
+        <v>67039</v>
       </c>
       <c r="D38">
         <v>31.96</v>
@@ -3891,10 +3936,10 @@
         <v>8.49</v>
       </c>
       <c r="F38">
-        <v>14538</v>
+        <v>52695</v>
       </c>
       <c r="G38">
-        <v>2.64333333333333</v>
+        <v>4.64333333333333</v>
       </c>
       <c r="H38">
         <v>1.29833333333333</v>
@@ -3917,10 +3962,10 @@
         <v>15</v>
       </c>
       <c r="B39">
-        <v>17982</v>
+        <v>71928</v>
       </c>
       <c r="C39">
-        <v>38408</v>
+        <v>99260</v>
       </c>
       <c r="D39">
         <v>46.626666666666601</v>
@@ -3929,10 +3974,10 @@
         <v>12.156666666666601</v>
       </c>
       <c r="F39">
-        <v>20675</v>
+        <v>76826</v>
       </c>
       <c r="G39">
-        <v>2.6966666666666601</v>
+        <v>4.6966666666666601</v>
       </c>
       <c r="H39">
         <v>1.3233333333333299</v>
@@ -3955,10 +4000,10 @@
         <v>20</v>
       </c>
       <c r="B40">
-        <v>23978</v>
+        <v>95912</v>
       </c>
       <c r="C40">
-        <v>50919</v>
+        <v>131678</v>
       </c>
       <c r="D40">
         <v>61.946666666666601</v>
@@ -3967,10 +4012,10 @@
         <v>15.986666666666601</v>
       </c>
       <c r="F40">
-        <v>26780</v>
+        <v>100920</v>
       </c>
       <c r="G40">
-        <v>2.6966666666666601</v>
+        <v>4.6966666666666601</v>
       </c>
       <c r="H40">
         <v>1.32</v>

</xml_diff>